<commit_message>
* Program.cs: * CSV.csproj: * Constants.cs: * test.docx: * FTP.cs: * logo.jpg: * students.csv: * students.xml: * ~$udents.docx: * students.xlsx: * MyImage.jpg: * students.pptx: * students.json: * students.docx: * ~$students.xlsx: * studentsapi.docx: * ~$udentsapi.docx: * StudentNewModel.cs: * StudentController.cs: * SpreadSheetClass.cs: * WordDocumentClass.cs: * PresentationClass.cs:
* ~$students.pptx: Final Commit with OPEN XML
</commit_message>
<xml_diff>
--- a/Content/Data/students.xlsx
+++ b/Content/Data/students.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R3eead65909bf455c"/>
-    <x:sheet name="Sheet2" sheetId="2" r:id="R1e2b72b45fbd43d4"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R37644197389f4863"/>
+    <x:sheet name="Sheet2" sheetId="2" r:id="Ra4f82f5bf9cf4af8"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -48,7 +48,7 @@
     </x:row>
     <x:row r="2">
       <x:c r="A2" t="str">
-        <x:v>d7cc687c-d8e2-45e2-bec9-5c157934ab0f</x:v>
+        <x:v>22c6338d-7c6d-4be6-8bb4-179734223f46</x:v>
       </x:c>
       <x:c r="B2" t="n">
         <x:v>200450333</x:v>
@@ -71,7 +71,7 @@
     </x:row>
     <x:row r="3">
       <x:c r="A3" t="str">
-        <x:v>ee7a0b50-f874-4064-88ac-70445ad6da4c</x:v>
+        <x:v>3567d5ab-a906-48fc-98ae-1e0e41f96766</x:v>
       </x:c>
       <x:c r="B3" t="n">
         <x:v>20033515</x:v>
@@ -94,7 +94,7 @@
     </x:row>
     <x:row r="4">
       <x:c r="A4" t="str">
-        <x:v>8138f5c3-c2e6-4664-bf3b-daaf6e61250d</x:v>
+        <x:v>d128f654-d4f5-43d9-a88f-09c6515bd382</x:v>
       </x:c>
       <x:c r="B4" t="n">
         <x:v>200423859</x:v>
@@ -117,7 +117,7 @@
     </x:row>
     <x:row r="5">
       <x:c r="A5" t="str">
-        <x:v>bcf8edf1-378e-4bf4-8067-0030d402c6c4</x:v>
+        <x:v>04e37b6a-f717-422f-84ea-48393bb0cda9</x:v>
       </x:c>
       <x:c r="B5" t="n">
         <x:v>200425031</x:v>
@@ -140,7 +140,7 @@
     </x:row>
     <x:row r="6">
       <x:c r="A6" t="str">
-        <x:v>30f770da-e4b7-4b83-bcef-911ecd23c72b</x:v>
+        <x:v>29a6198d-59a8-4754-93b3-d573156549ec</x:v>
       </x:c>
       <x:c r="B6" t="n">
         <x:v>200425170</x:v>
@@ -163,7 +163,7 @@
     </x:row>
     <x:row r="7">
       <x:c r="A7" t="str">
-        <x:v>f4a6bb9e-44a7-4050-a4e0-3b44df45ba53</x:v>
+        <x:v>55ff4e80-37b1-4649-966b-ae00317c38f5</x:v>
       </x:c>
       <x:c r="B7" t="n">
         <x:v>200425198</x:v>
@@ -186,7 +186,7 @@
     </x:row>
     <x:row r="8">
       <x:c r="A8" t="str">
-        <x:v>ca5583ee-5d75-410a-88db-17c6752ca841</x:v>
+        <x:v>e9b173db-16fc-44dc-88ed-655e90fb871a</x:v>
       </x:c>
       <x:c r="B8" t="n">
         <x:v>200427977</x:v>
@@ -209,7 +209,7 @@
     </x:row>
     <x:row r="9">
       <x:c r="A9" t="str">
-        <x:v>1e666ef5-17ab-49e6-83f4-f2dda71a8214</x:v>
+        <x:v>04fc89aa-f956-4079-9b67-2976eb3479a1</x:v>
       </x:c>
       <x:c r="B9" t="n">
         <x:v>200425898</x:v>
@@ -232,7 +232,7 @@
     </x:row>
     <x:row r="10">
       <x:c r="A10" t="str">
-        <x:v>1e57be58-ecc3-4f48-af12-37896e980d0b</x:v>
+        <x:v>eda5cd6c-ca97-43d3-aca5-3558e81f224f</x:v>
       </x:c>
       <x:c r="B10" t="n">
         <x:v>200427531</x:v>
@@ -251,6 +251,788 @@
       </x:c>
       <x:c r="G10" t="n">
         <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11">
+      <x:c r="A11" t="str">
+        <x:v>a9b64265-e52a-43dc-ad64-44fab8380d18</x:v>
+      </x:c>
+      <x:c r="B11" t="n">
+        <x:v>200427977</x:v>
+      </x:c>
+      <x:c r="C11" t="str">
+        <x:v>Mostafizur</x:v>
+      </x:c>
+      <x:c r="D11" t="str">
+        <x:v>Rahman</x:v>
+      </x:c>
+      <x:c r="E11" t="d">
+        <x:v>07/11/1994</x:v>
+      </x:c>
+      <x:c r="F11" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G11" t="n">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12">
+      <x:c r="A12" t="str">
+        <x:v>e644c884-4723-4d1f-ae77-fb15d192556e</x:v>
+      </x:c>
+      <x:c r="B12" t="n">
+        <x:v>200429013</x:v>
+      </x:c>
+      <x:c r="C12" t="str">
+        <x:v>Priyanka</x:v>
+      </x:c>
+      <x:c r="D12" t="str">
+        <x:v>Garg</x:v>
+      </x:c>
+      <x:c r="E12" t="d">
+        <x:v>12/09/1993</x:v>
+      </x:c>
+      <x:c r="F12" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G12" t="n">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13">
+      <x:c r="A13" t="str">
+        <x:v>1cbaac61-5873-4740-9069-93ad4dbb22a8</x:v>
+      </x:c>
+      <x:c r="B13" t="n">
+        <x:v>200429017</x:v>
+      </x:c>
+      <x:c r="C13" t="str">
+        <x:v>Manpreet</x:v>
+      </x:c>
+      <x:c r="D13" t="str">
+        <x:v>Kaur</x:v>
+      </x:c>
+      <x:c r="E13" t="d">
+        <x:v>10/27/1994</x:v>
+      </x:c>
+      <x:c r="F13" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G13" t="n">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14">
+      <x:c r="A14" t="str">
+        <x:v>b9c300cf-bd68-4df0-ab6d-e247469db815</x:v>
+      </x:c>
+      <x:c r="B14" t="n">
+        <x:v>200429019</x:v>
+      </x:c>
+      <x:c r="C14" t="str">
+        <x:v>Pranav</x:v>
+      </x:c>
+      <x:c r="D14" t="str">
+        <x:v>Sharma</x:v>
+      </x:c>
+      <x:c r="E14" t="d">
+        <x:v>09/19/1997</x:v>
+      </x:c>
+      <x:c r="F14" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G14" t="n">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15">
+      <x:c r="A15" t="str">
+        <x:v>3487d00b-3dc1-4808-8eb8-84fd85646f78</x:v>
+      </x:c>
+      <x:c r="B15" t="n">
+        <x:v>200429439</x:v>
+      </x:c>
+      <x:c r="C15" t="str">
+        <x:v>Kavya</x:v>
+      </x:c>
+      <x:c r="D15" t="str">
+        <x:v>Arora</x:v>
+      </x:c>
+      <x:c r="E15" t="d">
+        <x:v>09/08/1994</x:v>
+      </x:c>
+      <x:c r="F15" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G15" t="n">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16">
+      <x:c r="A16" t="str">
+        <x:v>b484038f-1526-4ac9-b164-7df02900e304</x:v>
+      </x:c>
+      <x:c r="B16" t="n">
+        <x:v>200429757</x:v>
+      </x:c>
+      <x:c r="C16" t="str">
+        <x:v>Aditya</x:v>
+      </x:c>
+      <x:c r="D16" t="str">
+        <x:v>Pidikiti</x:v>
+      </x:c>
+      <x:c r="E16" t="d">
+        <x:v/>
+      </x:c>
+      <x:c r="F16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G16" t="n">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17">
+      <x:c r="A17" t="str">
+        <x:v>32eac01c-17db-4605-b744-bb7310f72f1f</x:v>
+      </x:c>
+      <x:c r="B17" t="n">
+        <x:v>200430242</x:v>
+      </x:c>
+      <x:c r="C17" t="str">
+        <x:v>BalaPrathima</x:v>
+      </x:c>
+      <x:c r="D17" t="str">
+        <x:v>Gade</x:v>
+      </x:c>
+      <x:c r="E17" t="d">
+        <x:v>03/03/1996</x:v>
+      </x:c>
+      <x:c r="F17" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G17" t="n">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18">
+      <x:c r="A18" t="str">
+        <x:v>0406d90c-70e3-4fcc-8811-ce988bb28b69</x:v>
+      </x:c>
+      <x:c r="B18" t="n">
+        <x:v>200430858</x:v>
+      </x:c>
+      <x:c r="C18" t="str">
+        <x:v>Prajwal</x:v>
+      </x:c>
+      <x:c r="D18" t="str">
+        <x:v>Acharya</x:v>
+      </x:c>
+      <x:c r="E18" t="d">
+        <x:v/>
+      </x:c>
+      <x:c r="F18" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G18" t="n">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19">
+      <x:c r="A19" t="str">
+        <x:v>e7cba906-84f3-4fb2-b756-f50b1d37fa20</x:v>
+      </x:c>
+      <x:c r="B19" t="n">
+        <x:v>200439773</x:v>
+      </x:c>
+      <x:c r="C19" t="str">
+        <x:v>Preet</x:v>
+      </x:c>
+      <x:c r="D19" t="str">
+        <x:v>Shah</x:v>
+      </x:c>
+      <x:c r="E19" t="d">
+        <x:v>10/04/1998</x:v>
+      </x:c>
+      <x:c r="F19" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G19" t="n">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20">
+      <x:c r="A20" t="str">
+        <x:v>bce9641e-277f-4ec2-a5cc-233f223d0561</x:v>
+      </x:c>
+      <x:c r="B20" t="n">
+        <x:v>200439932</x:v>
+      </x:c>
+      <x:c r="C20" t="str">
+        <x:v>Bruno</x:v>
+      </x:c>
+      <x:c r="D20" t="str">
+        <x:v>Simoes</x:v>
+      </x:c>
+      <x:c r="E20" t="d">
+        <x:v>07/05/1976</x:v>
+      </x:c>
+      <x:c r="F20" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G20" t="n">
+        <x:v>44</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21">
+      <x:c r="A21" t="str">
+        <x:v>e644ba25-eced-4459-b6b9-9faf92a5982f</x:v>
+      </x:c>
+      <x:c r="B21" t="n">
+        <x:v>200443399</x:v>
+      </x:c>
+      <x:c r="C21" t="str">
+        <x:v>Tugrul</x:v>
+      </x:c>
+      <x:c r="D21" t="str">
+        <x:v>Goktas</x:v>
+      </x:c>
+      <x:c r="E21" t="d">
+        <x:v>10/08/1995</x:v>
+      </x:c>
+      <x:c r="F21" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G21" t="n">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22">
+      <x:c r="A22" t="str">
+        <x:v>7feb7088-118a-42dd-ba40-49391eb7b83f</x:v>
+      </x:c>
+      <x:c r="B22" t="n">
+        <x:v>200445913</x:v>
+      </x:c>
+      <x:c r="C22" t="str">
+        <x:v>Prajwal</x:v>
+      </x:c>
+      <x:c r="D22" t="str">
+        <x:v>Katuwal</x:v>
+      </x:c>
+      <x:c r="E22" t="d">
+        <x:v>7/16/1993</x:v>
+      </x:c>
+      <x:c r="F22" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G22" t="n">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23">
+      <x:c r="A23" t="str">
+        <x:v>5444ec40-b651-49d9-be95-285f97d42d2a</x:v>
+      </x:c>
+      <x:c r="B23" t="n">
+        <x:v>200446535</x:v>
+      </x:c>
+      <x:c r="C23" t="str">
+        <x:v>Pavel</x:v>
+      </x:c>
+      <x:c r="D23" t="str">
+        <x:v>Sazonov</x:v>
+      </x:c>
+      <x:c r="E23" t="d">
+        <x:v>03/20/1988</x:v>
+      </x:c>
+      <x:c r="F23" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G23" t="n">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24">
+      <x:c r="A24" t="str">
+        <x:v>d008d09f-c487-4945-a8f6-ec370330a9fa</x:v>
+      </x:c>
+      <x:c r="B24" t="n">
+        <x:v>2200447714</x:v>
+      </x:c>
+      <x:c r="C24" t="str">
+        <x:v>swarnim</x:v>
+      </x:c>
+      <x:c r="D24" t="str">
+        <x:v>sharma</x:v>
+      </x:c>
+      <x:c r="E24" t="d">
+        <x:v>01/05/2020</x:v>
+      </x:c>
+      <x:c r="F24" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G24" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25">
+      <x:c r="A25" t="str">
+        <x:v>cf3535b1-65a1-400e-8e66-1cb895a3580f</x:v>
+      </x:c>
+      <x:c r="B25" t="n">
+        <x:v>200443399</x:v>
+      </x:c>
+      <x:c r="C25" t="str">
+        <x:v>Tugrul</x:v>
+      </x:c>
+      <x:c r="D25" t="str">
+        <x:v>Goktas</x:v>
+      </x:c>
+      <x:c r="E25" t="d">
+        <x:v>10/08/1995</x:v>
+      </x:c>
+      <x:c r="F25" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G25" t="n">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26">
+      <x:c r="A26" t="str">
+        <x:v>ed54ed70-fb1d-478c-923b-27f5855b0413</x:v>
+      </x:c>
+      <x:c r="B26" t="n">
+        <x:v>200447184</x:v>
+      </x:c>
+      <x:c r="C26" t="str">
+        <x:v>Jay</x:v>
+      </x:c>
+      <x:c r="D26" t="str">
+        <x:v>Kalal</x:v>
+      </x:c>
+      <x:c r="E26" t="d">
+        <x:v>01/27/1998</x:v>
+      </x:c>
+      <x:c r="F26" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G26" t="n">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27">
+      <x:c r="A27" t="str">
+        <x:v>dbcd310d-6136-443d-b07a-fa090d28092c</x:v>
+      </x:c>
+      <x:c r="B27" t="n">
+        <x:v>200447197</x:v>
+      </x:c>
+      <x:c r="C27" t="str">
+        <x:v>HemaAbhinandu</x:v>
+      </x:c>
+      <x:c r="D27" t="str">
+        <x:v>Kotha</x:v>
+      </x:c>
+      <x:c r="E27" t="d">
+        <x:v>04-15-1997</x:v>
+      </x:c>
+      <x:c r="F27" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G27" t="n">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28">
+      <x:c r="A28" t="str">
+        <x:v>7560d894-3efb-4aac-9be3-f6fcabdc92fb</x:v>
+      </x:c>
+      <x:c r="B28" t="n">
+        <x:v>200447261</x:v>
+      </x:c>
+      <x:c r="C28" t="str">
+        <x:v>AkhilDas</x:v>
+      </x:c>
+      <x:c r="D28" t="str">
+        <x:v>PradeepKumar</x:v>
+      </x:c>
+      <x:c r="E28" t="d">
+        <x:v>07/04/1993</x:v>
+      </x:c>
+      <x:c r="F28" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G28" t="n">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29">
+      <x:c r="A29" t="str">
+        <x:v>5f3dc460-f9e9-4e8d-8186-da151f242769</x:v>
+      </x:c>
+      <x:c r="B29" t="n">
+        <x:v>200447330</x:v>
+      </x:c>
+      <x:c r="C29" t="str">
+        <x:v>Swathi</x:v>
+      </x:c>
+      <x:c r="D29" t="str">
+        <x:v>Palavalli</x:v>
+      </x:c>
+      <x:c r="E29" t="d">
+        <x:v>04/05/1992</x:v>
+      </x:c>
+      <x:c r="F29" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G29" t="n">
+        <x:v>28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30">
+      <x:c r="A30" t="str">
+        <x:v>9867881b-5313-44c3-ad2b-9244a6958d7f</x:v>
+      </x:c>
+      <x:c r="B30" t="n">
+        <x:v>200447599</x:v>
+      </x:c>
+      <x:c r="C30" t="str">
+        <x:v>KavirajSingh</x:v>
+      </x:c>
+      <x:c r="D30" t="str">
+        <x:v>Jon</x:v>
+      </x:c>
+      <x:c r="E30" t="d">
+        <x:v>9/22/1994</x:v>
+      </x:c>
+      <x:c r="F30" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G30" t="n">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31">
+      <x:c r="A31" t="str">
+        <x:v>1c5c887d-2f04-43b5-8f61-eddc7e3d64ba</x:v>
+      </x:c>
+      <x:c r="B31" t="n">
+        <x:v>200447744</x:v>
+      </x:c>
+      <x:c r="C31" t="str">
+        <x:v>Althaf</x:v>
+      </x:c>
+      <x:c r="D31" t="str">
+        <x:v>Edathara</x:v>
+      </x:c>
+      <x:c r="E31" t="d">
+        <x:v>05/10/1993</x:v>
+      </x:c>
+      <x:c r="F31" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G31" t="n">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32">
+      <x:c r="A32" t="str">
+        <x:v>50a51a6c-6385-4c48-b132-18fb0840ca5b</x:v>
+      </x:c>
+      <x:c r="B32" t="n">
+        <x:v>200447887</x:v>
+      </x:c>
+      <x:c r="C32" t="str">
+        <x:v>Nipin</x:v>
+      </x:c>
+      <x:c r="D32" t="str">
+        <x:v>Dasani</x:v>
+      </x:c>
+      <x:c r="E32" t="d">
+        <x:v>01/29/1998</x:v>
+      </x:c>
+      <x:c r="F32" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G32" t="n">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33">
+      <x:c r="A33" t="str">
+        <x:v>3b852994-ddfc-4859-9f52-21f052db3529</x:v>
+      </x:c>
+      <x:c r="B33" t="n">
+        <x:v>200448226</x:v>
+      </x:c>
+      <x:c r="C33" t="str">
+        <x:v>Avi</x:v>
+      </x:c>
+      <x:c r="D33" t="str">
+        <x:v>Saini</x:v>
+      </x:c>
+      <x:c r="E33" t="d">
+        <x:v/>
+      </x:c>
+      <x:c r="F33" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G33" t="n">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34">
+      <x:c r="A34" t="str">
+        <x:v>fc046fce-6c9e-4a10-af26-f534fb57da5f</x:v>
+      </x:c>
+      <x:c r="B34" t="n">
+        <x:v>200448232</x:v>
+      </x:c>
+      <x:c r="C34" t="str">
+        <x:v>Kashish</x:v>
+      </x:c>
+      <x:c r="D34" t="str">
+        <x:v>Jhaveri</x:v>
+      </x:c>
+      <x:c r="E34" t="d">
+        <x:v>12/26/1996</x:v>
+      </x:c>
+      <x:c r="F34" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G34" t="n">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35">
+      <x:c r="A35" t="str">
+        <x:v>234f1ac2-d187-4ea9-987f-b27440266658</x:v>
+      </x:c>
+      <x:c r="B35" t="n">
+        <x:v>200449068</x:v>
+      </x:c>
+      <x:c r="C35" t="str">
+        <x:v>Robert</x:v>
+      </x:c>
+      <x:c r="D35" t="str">
+        <x:v>Routledge</x:v>
+      </x:c>
+      <x:c r="E35" t="d">
+        <x:v>05/20/1980</x:v>
+      </x:c>
+      <x:c r="F35" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G35" t="n">
+        <x:v>40</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36">
+      <x:c r="A36" t="str">
+        <x:v>96008225-cfa5-4a9e-8c01-243e6bbfe6a2</x:v>
+      </x:c>
+      <x:c r="B36" t="n">
+        <x:v>200449112</x:v>
+      </x:c>
+      <x:c r="C36" t="str">
+        <x:v>Sahiba</x:v>
+      </x:c>
+      <x:c r="D36" t="str">
+        <x:v>Sachdeva</x:v>
+      </x:c>
+      <x:c r="E36" t="d">
+        <x:v>08/23/1994</x:v>
+      </x:c>
+      <x:c r="F36" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G36" t="n">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37">
+      <x:c r="A37" t="str">
+        <x:v>ca130657-5f17-4414-849b-44b8a14645e4</x:v>
+      </x:c>
+      <x:c r="B37" t="n">
+        <x:v>200449872</x:v>
+      </x:c>
+      <x:c r="C37" t="str">
+        <x:v>Sofiya</x:v>
+      </x:c>
+      <x:c r="D37" t="str">
+        <x:v>Raju</x:v>
+      </x:c>
+      <x:c r="E37" t="d">
+        <x:v>09/22/1993</x:v>
+      </x:c>
+      <x:c r="F37" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G37" t="n">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38">
+      <x:c r="A38" t="str">
+        <x:v>1135a38a-e599-42de-b157-1f60c9b36322</x:v>
+      </x:c>
+      <x:c r="B38" t="n">
+        <x:v>200450261</x:v>
+      </x:c>
+      <x:c r="C38" t="str">
+        <x:v>Sony</x:v>
+      </x:c>
+      <x:c r="D38" t="str">
+        <x:v>Varghese</x:v>
+      </x:c>
+      <x:c r="E38" t="d">
+        <x:v>04/15/1994</x:v>
+      </x:c>
+      <x:c r="F38" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G38" t="n">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39">
+      <x:c r="A39" t="str">
+        <x:v>04853180-033d-4020-ad65-1ca2813d9305</x:v>
+      </x:c>
+      <x:c r="B39" t="n">
+        <x:v>200450333</x:v>
+      </x:c>
+      <x:c r="C39" t="str">
+        <x:v>Krishnapriya</x:v>
+      </x:c>
+      <x:c r="D39" t="str">
+        <x:v>Sarojam</x:v>
+      </x:c>
+      <x:c r="E39" t="d">
+        <x:v>12/31/1992</x:v>
+      </x:c>
+      <x:c r="F39" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G39" t="n">
+        <x:v>28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40">
+      <x:c r="A40" t="str">
+        <x:v>d6fdc76c-21a3-4d70-a704-92ccbf411310</x:v>
+      </x:c>
+      <x:c r="B40" t="n">
+        <x:v>200450515</x:v>
+      </x:c>
+      <x:c r="C40" t="str">
+        <x:v>SargunSingh</x:v>
+      </x:c>
+      <x:c r="D40" t="str">
+        <x:v>Walia</x:v>
+      </x:c>
+      <x:c r="E40" t="d">
+        <x:v>07/18/1994</x:v>
+      </x:c>
+      <x:c r="F40" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G40" t="n">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41">
+      <x:c r="A41" t="str">
+        <x:v>b6827dd5-ac56-49df-b38a-42fc75122dbe</x:v>
+      </x:c>
+      <x:c r="B41" t="n">
+        <x:v>200450550</x:v>
+      </x:c>
+      <x:c r="C41" t="str">
+        <x:v>Nikhil</x:v>
+      </x:c>
+      <x:c r="D41" t="str">
+        <x:v>Patel</x:v>
+      </x:c>
+      <x:c r="E41" t="d">
+        <x:v>11/30/1997</x:v>
+      </x:c>
+      <x:c r="F41" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G41" t="n">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42">
+      <x:c r="A42" t="str">
+        <x:v>9a6a32e9-951e-4a34-b300-a92098bd8ddf</x:v>
+      </x:c>
+      <x:c r="B42" t="n">
+        <x:v>200450635</x:v>
+      </x:c>
+      <x:c r="C42" t="str">
+        <x:v>Gurminder</x:v>
+      </x:c>
+      <x:c r="D42" t="str">
+        <x:v>Singh</x:v>
+      </x:c>
+      <x:c r="E42" t="d">
+        <x:v>2/9/1997</x:v>
+      </x:c>
+      <x:c r="F42" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G42" t="n">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43">
+      <x:c r="A43" t="str">
+        <x:v>935b17d6-8405-4798-a391-c1d86570da3e</x:v>
+      </x:c>
+      <x:c r="B43" t="n">
+        <x:v>200450730</x:v>
+      </x:c>
+      <x:c r="C43" t="str">
+        <x:v>Vrunda</x:v>
+      </x:c>
+      <x:c r="D43" t="str">
+        <x:v>Patel</x:v>
+      </x:c>
+      <x:c r="E43" t="d">
+        <x:v/>
+      </x:c>
+      <x:c r="F43" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G43" t="n">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44">
+      <x:c r="A44" t="str">
+        <x:v>264c9484-53bb-43a5-a693-e73c29c0833d</x:v>
+      </x:c>
+      <x:c r="B44" t="n">
+        <x:v>200451605</x:v>
+      </x:c>
+      <x:c r="C44" t="str">
+        <x:v>Vrushabh</x:v>
+      </x:c>
+      <x:c r="D44" t="str">
+        <x:v>Patel</x:v>
+      </x:c>
+      <x:c r="E44" t="d">
+        <x:v>6/15/1996</x:v>
+      </x:c>
+      <x:c r="F44" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G44" t="n">
+        <x:v>24</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>